<commit_message>
Updated, refactored, and documented
</commit_message>
<xml_diff>
--- a/fourfactorsrawdata.xlsx
+++ b/fourfactorsrawdata.xlsx
@@ -58,25 +58,25 @@
     <t>OPP_OREB_PCT</t>
   </si>
   <si>
-    <t>0022000535</t>
-  </si>
-  <si>
-    <t>Trail Blazers</t>
-  </si>
-  <si>
-    <t>Hornets</t>
-  </si>
-  <si>
-    <t>POR</t>
-  </si>
-  <si>
-    <t>CHA</t>
-  </si>
-  <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
+    <t>0022000098</t>
+  </si>
+  <si>
+    <t>Rockets</t>
+  </si>
+  <si>
+    <t>Mavericks</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
   <si>
     <t>240:00</t>
@@ -495,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>1610612757</v>
+        <v>1610612745</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -510,28 +510,28 @@
         <v>21</v>
       </c>
       <c r="H2">
-        <v>0.674</v>
+        <v>0.461</v>
       </c>
       <c r="I2">
-        <v>0.116</v>
+        <v>0.468</v>
       </c>
       <c r="J2">
-        <v>0.171</v>
+        <v>0.123</v>
       </c>
       <c r="K2">
-        <v>0.2</v>
+        <v>0.137</v>
       </c>
       <c r="L2">
-        <v>0.574</v>
+        <v>0.573</v>
       </c>
       <c r="M2">
-        <v>0.193</v>
+        <v>0.244</v>
       </c>
       <c r="N2">
-        <v>0.159</v>
+        <v>0.182</v>
       </c>
       <c r="O2">
-        <v>0.306</v>
+        <v>0.326</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>1610612766</v>
+        <v>1610612742</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -557,28 +557,28 @@
         <v>21</v>
       </c>
       <c r="H3">
-        <v>0.574</v>
+        <v>0.573</v>
       </c>
       <c r="I3">
-        <v>0.193</v>
+        <v>0.244</v>
       </c>
       <c r="J3">
-        <v>0.159</v>
+        <v>0.182</v>
       </c>
       <c r="K3">
-        <v>0.224</v>
+        <v>0.233</v>
       </c>
       <c r="L3">
-        <v>0.674</v>
+        <v>0.461</v>
       </c>
       <c r="M3">
-        <v>0.116</v>
+        <v>0.468</v>
       </c>
       <c r="N3">
-        <v>0.171</v>
+        <v>0.123</v>
       </c>
       <c r="O3">
-        <v>0.275</v>
+        <v>0.176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved date issue '0#' --> '#'
</commit_message>
<xml_diff>
--- a/fourfactorsrawdata.xlsx
+++ b/fourfactorsrawdata.xlsx
@@ -58,25 +58,25 @@
     <t>OPP_OREB_PCT</t>
   </si>
   <si>
-    <t>0022000098</t>
-  </si>
-  <si>
-    <t>Rockets</t>
-  </si>
-  <si>
-    <t>Mavericks</t>
-  </si>
-  <si>
-    <t>HOU</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Dallas</t>
+    <t>0022000589</t>
+  </si>
+  <si>
+    <t>Wizards</t>
+  </si>
+  <si>
+    <t>Bucks</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
   </si>
   <si>
     <t>240:00</t>
@@ -495,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>1610612745</v>
+        <v>1610612764</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -510,28 +510,28 @@
         <v>21</v>
       </c>
       <c r="H2">
-        <v>0.461</v>
+        <v>0.543</v>
       </c>
       <c r="I2">
-        <v>0.468</v>
+        <v>0.234</v>
       </c>
       <c r="J2">
-        <v>0.123</v>
+        <v>0.133</v>
       </c>
       <c r="K2">
-        <v>0.137</v>
+        <v>0.113</v>
       </c>
       <c r="L2">
-        <v>0.573</v>
+        <v>0.52</v>
       </c>
       <c r="M2">
-        <v>0.244</v>
+        <v>0.253</v>
       </c>
       <c r="N2">
-        <v>0.182</v>
+        <v>0.157</v>
       </c>
       <c r="O2">
-        <v>0.326</v>
+        <v>0.286</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>1610612742</v>
+        <v>1610612749</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -557,28 +557,28 @@
         <v>21</v>
       </c>
       <c r="H3">
-        <v>0.573</v>
+        <v>0.52</v>
       </c>
       <c r="I3">
-        <v>0.244</v>
+        <v>0.253</v>
       </c>
       <c r="J3">
-        <v>0.182</v>
+        <v>0.157</v>
       </c>
       <c r="K3">
-        <v>0.233</v>
+        <v>0.232</v>
       </c>
       <c r="L3">
-        <v>0.461</v>
+        <v>0.543</v>
       </c>
       <c r="M3">
-        <v>0.468</v>
+        <v>0.234</v>
       </c>
       <c r="N3">
-        <v>0.123</v>
+        <v>0.133</v>
       </c>
       <c r="O3">
-        <v>0.176</v>
+        <v>0.151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>